<commit_message>
ADD ROW TO XLSX SERVICE
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
   <si>
     <t>Nama Karyawan</t>
   </si>
@@ -45,6 +45,93 @@
   </si>
   <si>
     <t>Bukti Foto Sesudah</t>
+  </si>
+  <si>
+    <t>hariachmad</t>
+  </si>
+  <si>
+    <t>sipil</t>
+  </si>
+  <si>
+    <t>Administrasi</t>
+  </si>
+  <si>
+    <t>09/03/2025</t>
+  </si>
+  <si>
+    <t>10:53:0011:55:00</t>
+  </si>
+  <si>
+    <t>administrasi</t>
+  </si>
+  <si>
+    <t>pending</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>08/03/2025</t>
+  </si>
+  <si>
+    <t>22:34:0023:35:00</t>
+  </si>
+  <si>
+    <t>ditolak</t>
+  </si>
+  <si>
+    <t>Head of Production</t>
+  </si>
+  <si>
+    <t>Sipil</t>
+  </si>
+  <si>
+    <t>06/03/2025</t>
+  </si>
+  <si>
+    <t>04:54:0008:58:00</t>
+  </si>
+  <si>
+    <t>disetujui</t>
+  </si>
+  <si>
+    <t>04:36:0005:36:00</t>
+  </si>
+  <si>
+    <t>sherlynn</t>
+  </si>
+  <si>
+    <t>furniture</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>06/02/2025</t>
+  </si>
+  <si>
+    <t>16:20:0018:30:00</t>
+  </si>
+  <si>
+    <t>HRGA Staff</t>
+  </si>
+  <si>
+    <t>lainnya</t>
+  </si>
+  <si>
+    <t>05/02/2025</t>
+  </si>
+  <si>
+    <t>15:50:0017:55:00</t>
+  </si>
+  <si>
+    <t>Co-Founder</t>
+  </si>
+  <si>
+    <t>01/02/2025</t>
+  </si>
+  <si>
+    <t>10:15:0012:25:00</t>
   </si>
 </sst>
 </file>
@@ -92,6 +179,311 @@
   <dxfs count="0"/>
   <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="476250" cy="95250"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1" name="Foto" descr="Foto"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="0"/>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="476250" cy="95250"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Foto" descr="Foto"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="0"/>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="476250" cy="95250"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Foto" descr="Foto"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="0"/>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="476250" cy="95250"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Foto" descr="Foto"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="0"/>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="476250" cy="95250"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Foto" descr="Foto"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="0"/>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="476250" cy="95250"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Foto" descr="Foto"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="0"/>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="476250" cy="95250"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Foto" descr="Foto"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="0"/>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="476250" cy="95250"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Foto" descr="Foto"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="0"/>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="476250" cy="95250"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Foto" descr="Foto"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="0"/>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="476250" cy="95250"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Foto" descr="Foto"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="0"/>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -384,15 +776,27 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="true" style="0"/>
+    <col min="2" max="2" width="18" customWidth="true" style="0"/>
+    <col min="3" max="3" width="18" customWidth="true" style="0"/>
+    <col min="4" max="4" width="22" customWidth="true" style="0"/>
+    <col min="5" max="5" width="22" customWidth="true" style="0"/>
+    <col min="6" max="6" width="22" customWidth="true" style="0"/>
+    <col min="7" max="7" width="10" customWidth="true" style="0"/>
+    <col min="8" max="8" width="20" customWidth="true" style="0"/>
+    <col min="9" max="9" width="22" customWidth="true" style="0"/>
+    <col min="14" max="14" width="22" customWidth="true" style="0"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -420,13 +824,222 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="N1" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>